<commit_message>
Added feature extraction script and several feature extraction functions. Enough to compute features to be used in classification for one sample file. Pending to read all sample files and concatenate them into a big eegTrainActvity set.
</commit_message>
<xml_diff>
--- a/FeatureExtraction.xlsx
+++ b/FeatureExtraction.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/danielvillarreal/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/DANFIT1/HifoCap/Matlab algorithms/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28800" yWindow="460" windowWidth="28800" windowHeight="16900" tabRatio="500"/>
+    <workbookView xWindow="-28800" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -214,31 +214,6 @@
     <t>Not directly implemented</t>
   </si>
   <si>
-    <r>
-      <t>feauture_names=TimeOffset,,,,AppEntropy,SampEntropy,,</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>,,,</t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="18"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Wavelet_db4_EnergyBand_1,Wavelet_db4_EnergyBand_2,Wavelet_db4_EnergyBand_3,Wavelet_db4_EnergyBand_4,Wavelet_db4_EnergyBand_5,Wavelet_db4_EnergyBand_6,</t>
-    </r>
-  </si>
-  <si>
     <t>f_sampen</t>
   </si>
   <si>
@@ -252,13 +227,16 @@
   </si>
   <si>
     <t>WaveletCoefficientEnergy</t>
+  </si>
+  <si>
+    <t>feauture_names=TimeOffset,,,,</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -275,13 +253,6 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
       <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -690,8 +661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="24" x14ac:dyDescent="0.3"/>
@@ -954,10 +925,10 @@
         <v>46</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="D15" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E15" s="12">
         <v>0</v>
@@ -972,10 +943,10 @@
         <v>45</v>
       </c>
       <c r="C16" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="D16" s="12" t="s">
         <v>51</v>
-      </c>
-      <c r="D16" s="12" t="s">
-        <v>52</v>
       </c>
       <c r="E16" s="12">
         <v>0</v>
@@ -990,10 +961,10 @@
         <v>15</v>
       </c>
       <c r="C17" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="D17" s="8" t="s">
         <v>53</v>
-      </c>
-      <c r="D17" s="8" t="s">
-        <v>54</v>
       </c>
       <c r="E17" s="8"/>
       <c r="F17" s="8"/>
@@ -1046,7 +1017,7 @@
         <v>41</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>